<commit_message>
view designed changes and layout modified
</commit_message>
<xml_diff>
--- a/documents/tables_design.xlsx
+++ b/documents/tables_design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Products</t>
   </si>
@@ -157,6 +157,39 @@
   </si>
   <si>
     <t>Balance</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>subtotal</t>
+  </si>
+  <si>
+    <t>shipping</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>payment_type</t>
+  </si>
+  <si>
+    <t>delivery_status</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>cod_orders</t>
+  </si>
+  <si>
+    <t>cod_order_details</t>
   </si>
 </sst>
 </file>
@@ -164,7 +197,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -207,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -286,18 +325,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,33 +646,41 @@
     <col min="13" max="13" width="10.453125" customWidth="1"/>
     <col min="14" max="14" width="14.90625" customWidth="1"/>
     <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="20" max="21" width="12.26953125" customWidth="1"/>
+    <col min="22" max="22" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:27" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="7"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -680,8 +734,16 @@
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -731,7 +793,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -777,24 +839,68 @@
       <c r="O5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="8" t="s">
+      <c r="S5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="S6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="W6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B8" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="5"/>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
       <c r="K8" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="V8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>2</v>
       </c>
@@ -810,7 +916,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
@@ -825,8 +931,26 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S10" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="W10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="X10" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
@@ -838,7 +962,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
@@ -848,7 +972,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
@@ -858,7 +982,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
@@ -868,7 +992,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
@@ -882,7 +1006,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
@@ -895,10 +1019,12 @@
       <c r="I16" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="G8:I8"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="V8:Z8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -909,7 +1035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -924,32 +1050,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -957,7 +1083,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>44562</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -976,7 +1102,7 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>44563</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -995,7 +1121,7 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="9">
         <v>44564</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1014,7 +1140,7 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>44565</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1033,7 +1159,7 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>44566</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1052,7 +1178,7 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="9">
         <v>44567</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1069,21 +1195,21 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
-      <c r="B9" s="11"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
         <f>SUM(F3:F8)-SUM(E3:E8)</f>
         <v>95000</v>
       </c>

</xml_diff>